<commit_message>
Updated material HP values
</commit_message>
<xml_diff>
--- a/FeedsandSpeeds_Rev1.xlsx
+++ b/FeedsandSpeeds_Rev1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tankh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tankh\Documents\GitHub\HEM_Feeds_and_Speeds_Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1924B3F9-E093-44AC-A281-3C8EC27C624B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B348CB43-47D1-4CC3-9FFA-02B9AF1F6208}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{085F0F65-DED3-4561-B200-39C5AB6CBB0D}"/>
   </bookViews>
@@ -32,22 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
-  <si>
-    <t>ALUMINUM</t>
-  </si>
-  <si>
-    <t>MAGNESIUM</t>
-  </si>
-  <si>
-    <t>COPPER</t>
-  </si>
-  <si>
-    <t>BRASS</t>
-  </si>
-  <si>
-    <t>BRONZE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>Material:</t>
   </si>
@@ -179,6 +164,48 @@
   </si>
   <si>
     <t>Created by Shelby Ryan</t>
+  </si>
+  <si>
+    <t>Gray Cast Iron</t>
+  </si>
+  <si>
+    <t>Ductile Cast Iron</t>
+  </si>
+  <si>
+    <t>Maleable Cast Iron</t>
+  </si>
+  <si>
+    <t>Chilled Cast Iron</t>
+  </si>
+  <si>
+    <t>High Tensile Alloys</t>
+  </si>
+  <si>
+    <t>Titanium</t>
+  </si>
+  <si>
+    <t>PH Series Stainless Steels</t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>Magnesium</t>
+  </si>
+  <si>
+    <t>Copper</t>
+  </si>
+  <si>
+    <t>Brass</t>
+  </si>
+  <si>
+    <t>Bronze</t>
+  </si>
+  <si>
+    <t>300 Series Stainless Steels</t>
+  </si>
+  <si>
+    <t>High Temp Alloys</t>
   </si>
 </sst>
 </file>
@@ -724,7 +751,7 @@
   <dimension ref="A1:U215"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,31 +767,31 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4">
         <v>0.375</v>
@@ -772,7 +799,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B6" s="11">
         <v>4</v>
@@ -780,7 +807,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B7" s="10">
         <v>600</v>
@@ -788,15 +815,15 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B9" s="4">
         <v>0.75</v>
@@ -804,7 +831,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B10" s="2">
         <v>1.5E-3</v>
@@ -812,7 +839,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2">
         <v>6000</v>
@@ -821,12 +848,12 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B13" s="14">
         <f>B7/(0.262*B5)</f>
@@ -835,7 +862,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B14" s="15">
         <f>((B5/2)/B22)^2*B10</f>
@@ -845,7 +872,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B15" s="15">
         <f>(B10*(B5/2))/SQRT((B5*B22)-B22^2)</f>
@@ -854,7 +881,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B16" s="15">
         <f>'Lookup Tables'!C11*Calculations!B5</f>
@@ -863,7 +890,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B17" s="15">
         <f>B16*B22*B20</f>
@@ -873,12 +900,12 @@
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B19" s="5">
         <f xml:space="preserve"> IF(B7/(0.262*B5)&gt;B11,B11,B7/(0.262*B5))</f>
@@ -887,7 +914,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B20" s="13">
         <f>B19*B6*B15</f>
@@ -896,7 +923,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B21" s="13">
         <f>0.35*B20</f>
@@ -905,7 +932,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B22" s="5">
         <f>B5*'Lookup Tables'!B11</f>
@@ -914,16 +941,16 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B23" s="12">
-        <f>B22*B9*B20*'Lookup Tables'!E10</f>
-        <v>0.34842514581591577</v>
+        <f>B22*B9*B20*'Lookup Tables'!E19</f>
+        <v>0.29035428817992981</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B24" s="12">
         <f>B9*B22*B20</f>
@@ -936,30 +963,30 @@
     </row>
     <row r="26" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B26" s="3"/>
     </row>
     <row r="27" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1174,7 +1201,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9B33EFF2-B2CC-4C93-B8BE-852D842C47D7}">
           <x14:formula1>
             <xm:f>'Lookup Tables'!$A$1:$A$10</xm:f>
@@ -1183,7 +1210,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9766C611-05C6-465B-9D0D-63914E19F83E}">
           <x14:formula1>
-            <xm:f>'Lookup Tables'!$D$1:$D$9</xm:f>
+            <xm:f>'Lookup Tables'!$D$1:$D$18</xm:f>
           </x14:formula1>
           <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
@@ -1195,21 +1222,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E08E49C-5DAD-42A4-93CF-5CE85DFD4D6B}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1">
         <v>0.05</v>
@@ -1218,15 +1245,15 @@
         <v>1.65</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="E1">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>0.1</v>
@@ -1235,15 +1262,15 @@
         <v>1.5</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="E2">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>0.15</v>
@@ -1252,7 +1279,7 @@
         <v>1.25</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="E3">
         <v>0.5</v>
@@ -1260,7 +1287,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>0.2</v>
@@ -1269,7 +1296,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="E4">
         <v>0.4</v>
@@ -1277,7 +1304,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>0.25</v>
@@ -1286,7 +1313,7 @@
         <v>0.75</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="E5">
         <v>0.5</v>
@@ -1294,7 +1321,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>0.3</v>
@@ -1303,7 +1330,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>1.4</v>
@@ -1311,7 +1338,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>0.35</v>
@@ -1320,7 +1347,7 @@
         <v>0.42499999999999999</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>1.7</v>
@@ -1328,7 +1355,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>0.4</v>
@@ -1337,7 +1364,7 @@
         <v>0.375</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -1345,7 +1372,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>0.35</v>
@@ -1354,7 +1381,7 @@
         <v>0.33</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E9">
         <v>2.5</v>
@@ -1362,7 +1389,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>0.5</v>
@@ -1370,9 +1397,11 @@
       <c r="C10">
         <v>0.16500000000000001</v>
       </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
       <c r="E10">
-        <f>VLOOKUP(Calculations!B4,D1:E9,2,0)</f>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1384,10 +1413,76 @@
         <f>VLOOKUP(Calculations!B8,A1:C10,3,0)</f>
         <v>1.65</v>
       </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11">
+        <v>0.56000000000000005</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f>VLOOKUP(Calculations!B4,D1:E18,2,0)</f>
+        <v>0.25</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Added basic set of instructions
</commit_message>
<xml_diff>
--- a/FeedsandSpeeds_Rev1.xlsx
+++ b/FeedsandSpeeds_Rev1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tankh\Documents\GitHub\HEM_Feeds_and_Speeds_Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE48FCA-DB37-4F98-B9C1-D1E0DE0406C7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11457337-7029-4923-BACF-6ADEAFEA66ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{085F0F65-DED3-4561-B200-39C5AB6CBB0D}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
   <si>
     <t>Material:</t>
   </si>
@@ -55,9 +55,6 @@
     <t xml:space="preserve">Surface Feet per Minute: </t>
   </si>
   <si>
-    <t>Radial Depth of Cut:</t>
-  </si>
-  <si>
     <t>RPM:</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>Output Variables:</t>
   </si>
   <si>
-    <t>Recommended Depth of Cut (in):</t>
-  </si>
-  <si>
     <t>Tool Diameter (in):</t>
   </si>
   <si>
@@ -203,6 +197,42 @@
   </si>
   <si>
     <t>High Temp Alloys</t>
+  </si>
+  <si>
+    <t>How to use HEM Fees and Speeds Calculator:</t>
+  </si>
+  <si>
+    <t>2. Enter the tool diameter in inches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Select the material you plan on maching from the drop down menu </t>
+  </si>
+  <si>
+    <t>3. Enter the number of flutes on your tool</t>
+  </si>
+  <si>
+    <t>4. Enter the correct SFM value for the given material from the SFM Look up chart</t>
+  </si>
+  <si>
+    <t>SFM Look Up Chart:</t>
+  </si>
+  <si>
+    <t>5. Select the radial width of cut from the drop down menu</t>
+  </si>
+  <si>
+    <t>Radial Width of Cut (% Tool Diameter):</t>
+  </si>
+  <si>
+    <t>6. Enter the desired axial depth of cut. If unkown, enter the value located in B16</t>
+  </si>
+  <si>
+    <t>Recommended Axial Depth of Cut (in):</t>
+  </si>
+  <si>
+    <t>7. Enter the chip load in inch per tooth. Refference B27 and B28 for more information</t>
+  </si>
+  <si>
+    <t>8. Enter the max RPM of your machine</t>
   </si>
 </sst>
 </file>
@@ -274,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -311,6 +341,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -333,15 +364,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>25023</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
+      <xdr:colOff>13817</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>22411</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>589174</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>30708</xdr:rowOff>
+      <xdr:colOff>577968</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>30707</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -369,7 +400,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3868641" y="22412"/>
+          <a:off x="3846229" y="212911"/>
           <a:ext cx="4127621" cy="7056796"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -747,35 +778,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318487D9-3DF9-422E-A87B-3126276F45BA}">
   <dimension ref="A1:U214"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="37" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" style="8" customWidth="1"/>
     <col min="4" max="4" width="26.5703125" style="8" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="8"/>
-    <col min="7" max="7" width="9.7109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="79" style="8" customWidth="1"/>
     <col min="8" max="21" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -783,15 +826,21 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="4">
         <v>0.375</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -801,6 +850,9 @@
       <c r="B6" s="11">
         <v>4</v>
       </c>
+      <c r="G6" s="16" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -809,26 +861,35 @@
       <c r="B7" s="10">
         <v>600</v>
       </c>
+      <c r="G7" s="16" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" s="4">
         <v>0.75</v>
       </c>
+      <c r="G9" s="16" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2">
         <v>1.5E-3</v>
@@ -836,7 +897,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2">
         <v>6000</v>
@@ -845,12 +906,12 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="14">
         <f>B7/(0.262*B5)</f>
@@ -859,50 +920,50 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="15">
         <f>((B5/2)/B22)^2*B10</f>
-        <v>0.14999999999999997</v>
+        <v>9.3749999999999979E-3</v>
       </c>
       <c r="J14"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" s="15">
         <f>(B10*(B5/2))/SQRT((B5*B22)-B22^2)</f>
-        <v>3.4412360080584266E-3</v>
+        <v>1.8749999999999999E-3</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B16" s="15">
         <f>'Lookup Tables'!C11*Calculations!B5</f>
-        <v>0.61874999999999991</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="15">
         <f>B16*B22*B20</f>
-        <v>0.95816915099376831</v>
+        <v>1.2656250000000002</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="5">
         <f xml:space="preserve"> IF(B7/(0.262*B5)&gt;B11,B11,B7/(0.262*B5))</f>
@@ -911,47 +972,47 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="13">
         <f>B19*B6*B15</f>
-        <v>82.589664193402243</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="13">
         <f>0.35*B20</f>
-        <v>28.906382467690783</v>
+        <v>15.749999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="5">
         <f>B5*'Lookup Tables'!B11</f>
-        <v>1.8750000000000003E-2</v>
+        <v>7.5000000000000011E-2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="12">
         <f>B22*B9*B20*'Lookup Tables'!E19</f>
-        <v>0.29035428817992981</v>
+        <v>0.63281250000000011</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="12">
         <f>B9*B22*B20</f>
-        <v>1.1614171527197192</v>
+        <v>2.5312500000000004</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -960,24 +1021,24 @@
     </row>
     <row r="26" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="3"/>
     </row>
     <row r="27" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1227,7 +1288,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1">
         <v>0.05</v>
@@ -1236,7 +1297,7 @@
         <v>1.65</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E1">
         <v>0.25</v>
@@ -1244,7 +1305,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0.1</v>
@@ -1253,7 +1314,7 @@
         <v>1.5</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E2">
         <v>0.25</v>
@@ -1261,7 +1322,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0.15</v>
@@ -1270,7 +1331,7 @@
         <v>1.25</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E3">
         <v>0.5</v>
@@ -1278,7 +1339,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>0.2</v>
@@ -1287,7 +1348,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4">
         <v>0.4</v>
@@ -1295,7 +1356,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>0.25</v>
@@ -1304,7 +1365,7 @@
         <v>0.75</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5">
         <v>0.5</v>
@@ -1312,7 +1373,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>0.3</v>
@@ -1329,7 +1390,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>0.35</v>
@@ -1346,7 +1407,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>0.4</v>
@@ -1363,7 +1424,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>0.35</v>
@@ -1380,7 +1441,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>0.5</v>
@@ -1389,7 +1450,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E10">
         <v>0.5</v>
@@ -1398,14 +1459,14 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <f>VLOOKUP(Calculations!B8,A1:B10,2,0)</f>
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="C11">
         <f>VLOOKUP(Calculations!B8,A1:C10,3,0)</f>
-        <v>1.65</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E11">
         <v>0.56000000000000005</v>
@@ -1415,7 +1476,7 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E12">
         <v>0.67</v>
@@ -1423,7 +1484,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E13">
         <v>1.67</v>
@@ -1431,7 +1492,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E14">
         <v>2.5</v>
@@ -1439,7 +1500,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E15">
         <v>1.67</v>
@@ -1447,7 +1508,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E16">
         <v>1.33</v>
@@ -1455,7 +1516,7 @@
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1463,7 +1524,7 @@
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E18">
         <v>2.5</v>

</xml_diff>